<commit_message>
completed output in excel file
fixed bugs; improved quality of dataset
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianm\Documents\GitHub\csDetector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97DA0D6-A705-49AA-9F66-26B41DC9B837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C03E02-48DA-46B1-A019-BD38052CFE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24456" yWindow="1032" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>repositoryUrl</t>
   </si>
@@ -37,40 +40,49 @@
     <t>OSE</t>
   </si>
   <si>
+    <t>PDE</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>TFS</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>https://github.com/tensorflow/ranking</t>
+  </si>
+  <si>
+    <t>ranking</t>
+  </si>
+  <si>
+    <t>tensorflow</t>
+  </si>
+  <si>
+    <t>12/03/2018</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>BCE</t>
-  </si>
-  <si>
-    <t>PDE</t>
-  </si>
-  <si>
-    <t>SV</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>TFS</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>adsasd</t>
-  </si>
-  <si>
-    <t>asasd</t>
   </si>
 </sst>
 </file>
@@ -86,12 +98,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,12 +111,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -116,7 +140,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -392,21 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,126 +446,128 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N10" s="1"/>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed adapter; cr1 in review
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -955,6 +955,81 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cr1 completed and approved
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -1030,6 +1030,531 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updatet web service with json response
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -1555,6 +1555,456 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented function to delete repo from disk
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -2005,6 +2005,981 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated delete repo functionality
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -2980,6 +2980,1581 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed delete repository function
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -4555,6 +4555,2706 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://github.com/Hironsan/anago</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>anago</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Hironsan</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>06/26/2017</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed output directory to allow concurrent calls
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -7255,6 +7255,2706 @@
         </is>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>https://github.com/microsoft/QuantumKatas</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>QuantumKatas</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>microsoft</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>06/06/2018</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>https://github.com/microsoft/QuantumKatas</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>QuantumKatas</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>microsoft</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>06/06/2018</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
file download api implemented
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:O158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -10855,6 +10855,1431 @@
         </is>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes in file upload
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O158"/>
+  <dimension ref="A1:O164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -12280,6 +12280,456 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improved web service to handle date
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O164"/>
+  <dimension ref="A1:O172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -12730,6 +12730,606 @@
         </is>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>01/12/2020</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>01/12/2020</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>01/12/2020</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>01/12/2020</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
method and variables names refactored
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O172"/>
+  <dimension ref="A1:O174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -13330,6 +13330,156 @@
         </is>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Now it is possible to analyze up to a certain date
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O172"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -13330,6 +13330,756 @@
         </is>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>https://github.com/rescrv/HyperDex</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>HyperDex</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>rescrv</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>04/13/2011</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>https://github.com/pocl/pocl</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>pocl</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>pocl</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>02/08/2011</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>https://github.com/raghakot/keras-vis</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>keras-vis</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>raghakot</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>11/11/2016</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>